<commit_message>
refactored login page and tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestData/TwitterData.xlsx
+++ b/src/test/resources/excelTestData/TwitterData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnt\eclipse-workspace\PageObjectModel\src\test\resources\excelTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\TwitterQA\src\test\resources\excelTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70F5E9D-E298-4FFE-B131-E2253326FC7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEBE065-B80E-4CB8-BBB1-C2E980AC2F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{458C0B33-4ABF-4A19-91B9-E275545BACC7}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>If we want to solve a problem that we have never solved before, we must leave the door to the unknown ajar. - richard feynman</t>
   </si>
   <si>
-    <t xml:space="preserve"> ashylarry</t>
-  </si>
-  <si>
     <t>I'm new to twitter! Hello world!</t>
   </si>
   <si>
@@ -68,16 +65,19 @@
     <t xml:space="preserve"> johndoetest1</t>
   </si>
   <si>
-    <t>john87546528</t>
-  </si>
-  <si>
-    <t>ashley48792978</t>
-  </si>
-  <si>
     <t xml:space="preserve"> john87546528</t>
   </si>
   <si>
     <t xml:space="preserve"> ashley48792978</t>
+  </si>
+  <si>
+    <t>james8928748234</t>
+  </si>
+  <si>
+    <t>Tommy82379834893</t>
+  </si>
+  <si>
+    <t>thomas798597241</t>
   </si>
 </sst>
 </file>
@@ -459,13 +459,13 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="3" width="27.44140625" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" customWidth="1"/>
     <col min="5" max="5" width="21.21875" customWidth="1"/>
@@ -494,42 +494,42 @@
     </row>
     <row r="2" spans="1:6" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>